<commit_message>
merubah file lapkeu bab4
</commit_message>
<xml_diff>
--- a/lapkeu bab 4 (Autosaved).xlsx
+++ b/lapkeu bab 4 (Autosaved).xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="33">
   <si>
     <t>AGRO</t>
   </si>
@@ -112,6 +111,9 @@
   </si>
   <si>
     <t>MAX</t>
+  </si>
+  <si>
+    <t>ssss</t>
   </si>
 </sst>
 </file>
@@ -241,8 +243,14 @@
     <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -263,12 +271,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -574,7 +576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
+    <sheetView topLeftCell="D9" workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -586,73 +588,73 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="L2" s="21" t="s">
+      <c r="D2" s="13"/>
+      <c r="L2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="21"/>
+      <c r="M2" s="13"/>
       <c r="N2" s="1"/>
-      <c r="T2" s="21" t="s">
+      <c r="T2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="21"/>
+      <c r="U2" s="13"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
       <c r="N3" s="1"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
     </row>
     <row r="4" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="J4" s="19" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="J4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="R4" s="20" t="s">
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="R4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="S4" s="20" t="s">
+      <c r="S4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="T4" s="20" t="s">
+      <c r="T4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="U4" s="20"/>
-      <c r="V4" s="20"/>
-      <c r="W4" s="20"/>
-      <c r="X4" s="20"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="5">
         <v>2018</v>
       </c>
@@ -668,8 +670,8 @@
       <c r="G5" s="5">
         <v>2022</v>
       </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
       <c r="L5" s="4">
         <v>2018</v>
       </c>
@@ -685,8 +687,8 @@
       <c r="P5" s="4">
         <v>2022</v>
       </c>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
       <c r="T5" s="6">
         <v>2018</v>
       </c>
@@ -2199,10 +2201,10 @@
       </c>
     </row>
     <row r="29" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="15"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="10">
         <f>AVERAGE(C6:C28)</f>
         <v>0.89121739130434774</v>
@@ -2223,10 +2225,10 @@
         <f>AVERAGE(G6:G28)</f>
         <v>0.8406652173913044</v>
       </c>
-      <c r="J29" s="13" t="s">
+      <c r="J29" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="K29" s="13"/>
+      <c r="K29" s="15"/>
       <c r="L29" s="9">
         <f>AVERAGE(L6:L28)</f>
         <v>5.1726086956521741E-2</v>
@@ -2247,10 +2249,10 @@
         <f>AVERAGE(P6:P28)</f>
         <v>4.8404347826086956E-2</v>
       </c>
-      <c r="R29" s="12" t="s">
+      <c r="R29" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="S29" s="12"/>
+      <c r="S29" s="21"/>
       <c r="T29" s="11">
         <f>AVERAGE(T6:T28)</f>
         <v>1.1530434782608697E-2</v>
@@ -2273,10 +2275,10 @@
       </c>
     </row>
     <row r="30" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="17"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="10">
         <f>MIN(C6:C28)</f>
         <v>0.51959999999999995</v>
@@ -2297,10 +2299,10 @@
         <f>MIN(G6:G28)</f>
         <v>0.20530000000000001</v>
       </c>
-      <c r="J30" s="13" t="s">
+      <c r="J30" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K30" s="13"/>
+      <c r="K30" s="15"/>
       <c r="L30" s="9">
         <f>MIN(L6:L28)</f>
         <v>1.8200000000000001E-2</v>
@@ -2321,10 +2323,10 @@
         <f>MIN(P6:P28)</f>
         <v>-2.3300000000000001E-2</v>
       </c>
-      <c r="R30" s="12" t="s">
+      <c r="R30" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="S30" s="12"/>
+      <c r="S30" s="21"/>
       <c r="T30" s="11">
         <f>MIN(T6:T28)</f>
         <v>-2.8299999999999999E-2</v>
@@ -2347,10 +2349,10 @@
       </c>
     </row>
     <row r="31" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="17"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="10">
         <f>MAX(C6:C28)</f>
         <v>1.1492</v>
@@ -2371,10 +2373,10 @@
         <f>MAX(G6:G28)</f>
         <v>1.4605999999999999</v>
       </c>
-      <c r="J31" s="13" t="s">
+      <c r="J31" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="13"/>
+      <c r="K31" s="15"/>
       <c r="L31" s="9">
         <f>MAX(L6:L28)</f>
         <v>0.113</v>
@@ -2395,10 +2397,10 @@
         <f>MAX(P6:P28)</f>
         <v>0.13830000000000001</v>
       </c>
-      <c r="R31" s="12" t="s">
+      <c r="R31" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="S31" s="12"/>
+      <c r="S31" s="21"/>
       <c r="T31" s="11">
         <f>MAX(T6:T28)</f>
         <v>3.6799999999999999E-2</v>
@@ -2422,6 +2424,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="T4:X4"/>
     <mergeCell ref="C2:D3"/>
     <mergeCell ref="T2:U3"/>
@@ -2432,17 +2445,6 @@
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="R4:R5"/>
     <mergeCell ref="S4:S5"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J31:K31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2453,10 +2455,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
menambahkan kesimpulan dan membuat file saran
</commit_message>
<xml_diff>
--- a/lapkeu bab 4 (Autosaved).xlsx
+++ b/lapkeu bab 4 (Autosaved).xlsx
@@ -221,14 +221,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -239,24 +245,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" topLeftCell="L22" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,73 +575,73 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="L2" s="18" t="s">
+      <c r="D2" s="22"/>
+      <c r="L2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="18"/>
+      <c r="M2" s="22"/>
       <c r="N2" s="1"/>
-      <c r="T2" s="18" t="s">
+      <c r="T2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="18"/>
+      <c r="U2" s="22"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
       <c r="N3" s="1"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
     </row>
     <row r="4" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="J4" s="19" t="s">
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="J4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="R4" s="17" t="s">
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="R4" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="S4" s="17" t="s">
+      <c r="S4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="T4" s="17" t="s">
+      <c r="T4" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-      <c r="W4" s="17"/>
-      <c r="X4" s="17"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="5">
         <v>2018</v>
       </c>
@@ -657,8 +657,8 @@
       <c r="G5" s="5">
         <v>2022</v>
       </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
       <c r="L5" s="4">
         <v>2018</v>
       </c>
@@ -674,8 +674,8 @@
       <c r="P5" s="4">
         <v>2022</v>
       </c>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
       <c r="T5" s="6">
         <v>2018</v>
       </c>
@@ -2188,34 +2188,34 @@
       </c>
     </row>
     <row r="29" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="22">
+      <c r="B29" s="25"/>
+      <c r="C29" s="15">
         <f>AVERAGE(C6:C28)</f>
         <v>0.89121739130434774</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="15">
         <f>AVERAGE(D6:D28)</f>
         <v>0.91355217391304322</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29" s="15">
         <f>AVERAGE(E6:E28)</f>
         <v>0.83461304347826082</v>
       </c>
-      <c r="F29" s="22">
+      <c r="F29" s="15">
         <f>AVERAGE(F6:F28)</f>
         <v>0.82583043478260865</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G29" s="15">
         <f>AVERAGE(G6:G28)</f>
         <v>0.8406652173913044</v>
       </c>
-      <c r="J29" s="15" t="s">
+      <c r="J29" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="K29" s="15"/>
+      <c r="K29" s="24"/>
       <c r="L29" s="9">
         <f>AVERAGE(L6:L28)</f>
         <v>5.1726086956521741E-2</v>
@@ -2236,10 +2236,10 @@
         <f>AVERAGE(P6:P28)</f>
         <v>4.8404347826086956E-2</v>
       </c>
-      <c r="R29" s="14" t="s">
+      <c r="R29" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="S29" s="14"/>
+      <c r="S29" s="27"/>
       <c r="T29" s="10">
         <f>AVERAGE(T6:T28)</f>
         <v>1.1530434782608697E-2</v>
@@ -2262,34 +2262,34 @@
       </c>
     </row>
     <row r="30" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="22">
+      <c r="B30" s="25"/>
+      <c r="C30" s="15">
         <f>MIN(C6:C28)</f>
         <v>0.51959999999999995</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30" s="15">
         <f>MIN(D6:D28)</f>
         <v>0.48770000000000002</v>
       </c>
-      <c r="E30" s="22">
+      <c r="E30" s="15">
         <f>MIN(E6:E28)</f>
         <v>0.39329999999999998</v>
       </c>
-      <c r="F30" s="22">
+      <c r="F30" s="15">
         <f>MIN(F6:F28)</f>
         <v>0.1235</v>
       </c>
-      <c r="G30" s="22">
+      <c r="G30" s="15">
         <f>MIN(G6:G28)</f>
         <v>0.20530000000000001</v>
       </c>
-      <c r="J30" s="15" t="s">
+      <c r="J30" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="K30" s="15"/>
+      <c r="K30" s="24"/>
       <c r="L30" s="9">
         <f>MIN(L6:L28)</f>
         <v>1.8200000000000001E-2</v>
@@ -2310,10 +2310,10 @@
         <f>MIN(P6:P28)</f>
         <v>-2.3300000000000001E-2</v>
       </c>
-      <c r="R30" s="14" t="s">
+      <c r="R30" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="S30" s="14"/>
+      <c r="S30" s="27"/>
       <c r="T30" s="10">
         <f>MIN(T6:T28)</f>
         <v>-2.8299999999999999E-2</v>
@@ -2336,34 +2336,34 @@
       </c>
     </row>
     <row r="31" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="22">
+      <c r="B31" s="25"/>
+      <c r="C31" s="15">
         <f>MAX(C6:C28)</f>
         <v>1.1492</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="15">
         <f>MAX(D6:D28)</f>
         <v>1.63</v>
       </c>
-      <c r="E31" s="22">
+      <c r="E31" s="15">
         <f>MAX(E6:E28)</f>
         <v>1.4677</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F31" s="15">
         <f>MAX(F6:F28)</f>
         <v>2.2401</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G31" s="15">
         <f>MAX(G6:G28)</f>
         <v>1.4605999999999999</v>
       </c>
-      <c r="J31" s="15" t="s">
+      <c r="J31" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="15"/>
+      <c r="K31" s="24"/>
       <c r="L31" s="9">
         <f>MAX(L6:L28)</f>
         <v>0.113</v>
@@ -2384,10 +2384,10 @@
         <f>MAX(P6:P28)</f>
         <v>0.13830000000000001</v>
       </c>
-      <c r="R31" s="14" t="s">
+      <c r="R31" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="S31" s="14"/>
+      <c r="S31" s="27"/>
       <c r="T31" s="10">
         <f>MAX(T6:T28)</f>
         <v>3.6799999999999999E-2</v>
@@ -2410,27 +2410,27 @@
       </c>
     </row>
     <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G32" s="21" t="s">
+      <c r="G32" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="J32" s="24" t="s">
+      <c r="J32" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
       <c r="N32" s="13" t="s">
         <v>29</v>
       </c>
@@ -2440,12 +2440,12 @@
       <c r="P32" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="R32" s="26" t="s">
+      <c r="R32" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="S32" s="26"/>
-      <c r="T32" s="26"/>
-      <c r="U32" s="26"/>
+      <c r="S32" s="20"/>
+      <c r="T32" s="20"/>
+      <c r="U32" s="20"/>
       <c r="V32" s="12" t="s">
         <v>29</v>
       </c>
@@ -2457,57 +2457,65 @@
       </c>
     </row>
     <row r="33" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="22">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="15">
         <f>AVERAGE(C29:G29)</f>
         <v>0.86117565217391301</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F33" s="15">
         <f>MIN(C30:G30)</f>
         <v>0.1235</v>
       </c>
-      <c r="G33" s="22">
+      <c r="G33" s="15">
         <f>MAX(C31:G31)</f>
         <v>2.2401</v>
       </c>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="25">
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="16">
         <f>AVERAGE(L29:P29)</f>
         <v>4.474782608695653E-2</v>
       </c>
-      <c r="O33" s="25">
+      <c r="O33" s="16">
         <f>MIN(L30:P30)</f>
         <v>-3.5200000000000002E-2</v>
       </c>
-      <c r="P33" s="25">
+      <c r="P33" s="16">
         <f>MAX(L31:P31)</f>
         <v>0.13830000000000001</v>
       </c>
-      <c r="R33" s="26"/>
-      <c r="S33" s="26"/>
-      <c r="T33" s="26"/>
-      <c r="U33" s="26"/>
-      <c r="V33" s="27">
+      <c r="R33" s="20"/>
+      <c r="S33" s="20"/>
+      <c r="T33" s="20"/>
+      <c r="U33" s="20"/>
+      <c r="V33" s="17">
         <f>AVERAGE(T29:X29)</f>
         <v>6.4739130434782622E-3</v>
       </c>
-      <c r="W33" s="27">
+      <c r="W33" s="17">
         <f>MIN(T30:X30)</f>
         <v>-0.14749999999999999</v>
       </c>
-      <c r="X33" s="27">
+      <c r="X33" s="17">
         <f>MAX(T31:X31)</f>
         <v>4.2200000000000001E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J31:K31"/>
     <mergeCell ref="A32:D33"/>
     <mergeCell ref="J32:M33"/>
     <mergeCell ref="R32:U33"/>
@@ -2524,14 +2532,6 @@
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="R30:S30"/>
-    <mergeCell ref="R31:S31"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J31:K31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>